<commit_message>
Updated requirement files: new enemy requirement, logging
</commit_message>
<xml_diff>
--- a/requirements_realization.xlsx
+++ b/requirements_realization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Praktikum_CG\PGTD_Git\Game-Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beb\Documents\GitHub\Game-Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADB61CF-F0E7-4D22-A4F8-B02C8C039CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A53BB0B-2F42-44E0-B9BC-E846D9F9AB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2730" windowWidth="29040" windowHeight="15840" xr2:uid="{5A827F58-CBB4-425F-A3F7-4C3FD5A4CD13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A827F58-CBB4-425F-A3F7-4C3FD5A4CD13}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
   <si>
     <t>Realization</t>
   </si>
@@ -245,9 +245,6 @@
     <t>2h</t>
   </si>
   <si>
-    <t>including creating the first map and UI-Elements, spawnrate is adjustable</t>
-  </si>
-  <si>
     <t>Adjust the Spawnrate for each wave</t>
   </si>
   <si>
@@ -264,6 +261,28 @@
   </si>
   <si>
     <t>armor and resistance missing, different types of enemy</t>
+  </si>
+  <si>
+    <t>30h</t>
+  </si>
+  <si>
+    <t>including creating the first map and UI-Elements, 
+spawnrate is adjustable</t>
+  </si>
+  <si>
+    <t>2h +3h</t>
+  </si>
+  <si>
+    <t>Jonas + Ben</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>Ben + Jonas</t>
+  </si>
+  <si>
+    <t>2.5h</t>
   </si>
 </sst>
 </file>
@@ -635,21 +654,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D049B41F-43A8-48BF-BAB9-A1E45E86656D}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
     <col min="9" max="9" width="22.140625" customWidth="1"/>
     <col min="10" max="10" width="34" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
@@ -701,7 +720,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
         <v>65</v>
@@ -729,8 +748,8 @@
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>67</v>
+      <c r="E3" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="F3" t="s">
         <v>64</v>
@@ -745,7 +764,7 @@
         <v>63</v>
       </c>
       <c r="J3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K3" t="s">
         <v>39</v>
@@ -756,19 +775,19 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" t="s">
-        <v>70</v>
-      </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="I4" t="s">
         <v>63</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -802,39 +821,48 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -842,7 +870,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -850,7 +878,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
@@ -858,7 +886,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -866,7 +894,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -874,7 +902,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
@@ -882,44 +910,38 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>41</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G18" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="J17" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
       </c>
       <c r="J18" t="s">
         <v>37</v>
@@ -928,24 +950,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="J19" t="s">
         <v>37</v>
@@ -956,10 +966,10 @@
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>43</v>
@@ -968,13 +978,10 @@
         <v>41</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J20" t="s">
         <v>37</v>
@@ -983,24 +990,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G21" t="s">
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="J21" t="s">
         <v>37</v>
@@ -1011,55 +1021,70 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>52</v>
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
       </c>
       <c r="J22" t="s">
         <v>37</v>
       </c>
       <c r="K22" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="s">
+        <v>53</v>
       </c>
       <c r="J23" t="s">
         <v>37</v>
       </c>
       <c r="K23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -1070,20 +1095,43 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="F27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>